<commit_message>
Rendu de la version finale de l'application + mise à jour de l'autoévaluation
</commit_message>
<xml_diff>
--- a/Livrables/AutoEval_Greppin_Sam.xlsx
+++ b/Livrables/AutoEval_Greppin_Sam.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samgreppin\Desktop\SpacyNvader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theba\Desktop\SpacyNvader\Livrables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B2FF07-BDE7-4980-BDC0-CA774ABE4330}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CABBE6-8F43-4315-B3E1-343D9EEDFFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1585,6 +1585,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1610,83 +1687,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2327,7 +2327,7 @@
   <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="M19" sqref="M19:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
@@ -2369,11 +2369,11 @@
       <c r="M1" s="4"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="196" t="s">
+      <c r="P1" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="196"/>
-      <c r="R1" s="196"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="37.5" customHeight="1">
@@ -2461,14 +2461,14 @@
       <c r="M4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="197" t="str">
+      <c r="N4" s="173" t="str">
         <f>[1]Automation!F12</f>
         <v>29.8.2022 - 9.1.2023</v>
       </c>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
+      <c r="O4" s="173"/>
+      <c r="P4" s="173"/>
+      <c r="Q4" s="173"/>
+      <c r="R4" s="173"/>
       <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2508,34 +2508,34 @@
     <row r="7" spans="1:23" s="50" customFormat="1" ht="70.150000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="49"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="198" t="str">
+      <c r="E7" s="174" t="str">
         <f>[1]INDICATEURS!E7</f>
         <v>LARGEMENT ACQUIS
 5.5 ou 6.0</v>
       </c>
-      <c r="F7" s="199"/>
-      <c r="G7" s="199"/>
-      <c r="H7" s="200" t="str">
+      <c r="F7" s="175"/>
+      <c r="G7" s="175"/>
+      <c r="H7" s="176" t="str">
         <f>[1]INDICATEURS!H7</f>
         <v>SUFFISANT
 4.0, 4.5 ou 5.0</v>
       </c>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="202" t="str">
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="178" t="str">
         <f>[1]INDICATEURS!K7</f>
         <v>INSUFFISANT
 2.5, 3.0 ou 3.5</v>
       </c>
-      <c r="L7" s="203"/>
-      <c r="M7" s="203"/>
-      <c r="N7" s="204" t="str">
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="180" t="str">
         <f>[1]INDICATEURS!N7</f>
         <v>NON ACQUIS
 1.0, 1.5, ou 2.0</v>
       </c>
-      <c r="O7" s="205"/>
-      <c r="P7" s="205"/>
+      <c r="O7" s="181"/>
+      <c r="P7" s="181"/>
       <c r="Q7" s="52" t="str">
         <f>[1]INDICATEURS!Q7</f>
         <v>Coeff.</v>
@@ -2549,11 +2549,11 @@
     </row>
     <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="184" t="str">
+      <c r="B8" s="182" t="str">
         <f>[1]INDICATEURS!B8</f>
         <v>COMPÉTENCES</v>
       </c>
-      <c r="C8" s="187" t="str">
+      <c r="C8" s="185" t="str">
         <f>[1]INDICATEURS!C8</f>
         <v>PROFESSIONNELLES</v>
       </c>
@@ -2609,8 +2609,8 @@
     </row>
     <row r="9" spans="1:23" ht="100.15" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="185"/>
-      <c r="C9" s="188"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="186"/>
       <c r="D9" s="71" t="str">
         <f>[1]INDICATEURS!D9</f>
         <v>Conscience professionnelle
@@ -2624,9 +2624,7 @@
         <f>[1]INDICATEURS!F9</f>
         <v>Produit un travail parfaitement utilisable et transmissible sans retouches</v>
       </c>
-      <c r="G9" s="74">
-        <v>5.5</v>
-      </c>
+      <c r="G9" s="74"/>
       <c r="H9" s="75" t="s">
         <v>9</v>
       </c>
@@ -2634,7 +2632,9 @@
         <f>[1]INDICATEURS!I9</f>
         <v>Produit un travail utilisable, et transmissible, moyennant quelques retouches</v>
       </c>
-      <c r="J9" s="77"/>
+      <c r="J9" s="77">
+        <v>4</v>
+      </c>
       <c r="K9" s="78" t="s">
         <v>9</v>
       </c>
@@ -2657,14 +2657,14 @@
       </c>
       <c r="R9" s="85">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="185"/>
-      <c r="C10" s="188"/>
+      <c r="B10" s="183"/>
+      <c r="C10" s="186"/>
       <c r="D10" s="71" t="str">
         <f>[1]INDICATEURS!D10</f>
         <v>Connaissances professionnelles
@@ -2717,8 +2717,8 @@
     </row>
     <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="185"/>
-      <c r="C11" s="189" t="str">
+      <c r="B11" s="183"/>
+      <c r="C11" s="187" t="str">
         <f>[1]INDICATEURS!C11</f>
         <v>METHODOLOGIQUES</v>
       </c>
@@ -2773,8 +2773,8 @@
     </row>
     <row r="12" spans="1:23" ht="100.15" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="185"/>
-      <c r="C12" s="190"/>
+      <c r="B12" s="183"/>
+      <c r="C12" s="188"/>
       <c r="D12" s="102" t="str">
         <f>[1]INDICATEURS!D12</f>
         <v>Expression orale et écrite
@@ -2827,8 +2827,8 @@
     </row>
     <row r="13" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="185"/>
-      <c r="C13" s="191"/>
+      <c r="B13" s="183"/>
+      <c r="C13" s="189"/>
       <c r="D13" s="117" t="str">
         <f>[1]INDICATEURS!D13</f>
         <v>Approche écologique et économique
@@ -2881,7 +2881,7 @@
     </row>
     <row r="14" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="185"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="128" t="str">
         <f>[1]INDICATEURS!C14</f>
         <v>SOCIALES</v>
@@ -2899,7 +2899,7 @@
         <v>Influence positivement le groupe, manifeste un esprit entreprenant, constructif et cherche des solutions</v>
       </c>
       <c r="G14" s="119">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="87" t="s">
         <v>9</v>
@@ -2932,13 +2932,13 @@
       </c>
       <c r="R14" s="135">
         <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:23" ht="120" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="186"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="128" t="str">
         <f>[1]INDICATEURS!C15</f>
         <v>PERSONNELLES</v>
@@ -2966,7 +2966,7 @@
         <v>A parfois besoin d'aide (justifiée), fait ce qui est attendu de sa personne</v>
       </c>
       <c r="J15" s="142">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="K15" s="143" t="s">
         <v>9</v>
@@ -2990,7 +2990,7 @@
       </c>
       <c r="R15" s="135">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="S15" s="13"/>
     </row>
@@ -3012,7 +3012,7 @@
       <c r="M17" s="151"/>
       <c r="N17" s="153"/>
       <c r="O17" s="154"/>
-      <c r="P17" s="192" t="s">
+      <c r="P17" s="190" t="s">
         <v>11</v>
       </c>
       <c r="Q17" s="155"/>
@@ -3028,45 +3028,45 @@
       <c r="M18" s="152"/>
       <c r="N18" s="152"/>
       <c r="O18" s="152"/>
-      <c r="P18" s="192"/>
+      <c r="P18" s="190"/>
       <c r="Q18" s="155"/>
       <c r="R18" s="155"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="193"/>
-      <c r="C19" s="193"/>
-      <c r="D19" s="193"/>
-      <c r="E19" s="193"/>
-      <c r="F19" s="193"/>
-      <c r="G19" s="193"/>
-      <c r="H19" s="193"/>
-      <c r="I19" s="193"/>
-      <c r="K19" s="194" t="s">
+      <c r="B19" s="191"/>
+      <c r="C19" s="191"/>
+      <c r="D19" s="191"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="191"/>
+      <c r="I19" s="191"/>
+      <c r="K19" s="192" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="194"/>
-      <c r="M19" s="195">
-        <v>44893</v>
-      </c>
-      <c r="N19" s="195"/>
-      <c r="O19" s="195"/>
-      <c r="P19" s="192"/>
+      <c r="L19" s="192"/>
+      <c r="M19" s="193">
+        <v>44931</v>
+      </c>
+      <c r="N19" s="193"/>
+      <c r="O19" s="193"/>
+      <c r="P19" s="190"/>
       <c r="Q19" s="155"/>
       <c r="R19" s="155"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
+      <c r="B20" s="194"/>
+      <c r="C20" s="194"/>
+      <c r="D20" s="194"/>
+      <c r="E20" s="194"/>
+      <c r="F20" s="194"/>
+      <c r="G20" s="194"/>
+      <c r="H20" s="194"/>
+      <c r="I20" s="194"/>
       <c r="K20" s="158"/>
       <c r="L20" s="158"/>
       <c r="M20" s="152"/>
@@ -3079,23 +3079,23 @@
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="181"/>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="K21" s="182" t="s">
+      <c r="B21" s="194"/>
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
+      <c r="G21" s="194"/>
+      <c r="H21" s="194"/>
+      <c r="I21" s="194"/>
+      <c r="K21" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="182"/>
-      <c r="M21" s="183" t="s">
+      <c r="L21" s="195"/>
+      <c r="M21" s="196" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="183"/>
-      <c r="O21" s="183"/>
+      <c r="N21" s="196"/>
+      <c r="O21" s="196"/>
       <c r="P21" s="161"/>
       <c r="Q21" s="162"/>
       <c r="R21" s="162"/>
@@ -3103,14 +3103,14 @@
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="181"/>
-      <c r="C22" s="181"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
+      <c r="B22" s="194"/>
+      <c r="C22" s="194"/>
+      <c r="D22" s="194"/>
+      <c r="E22" s="194"/>
+      <c r="F22" s="194"/>
+      <c r="G22" s="194"/>
+      <c r="H22" s="194"/>
+      <c r="I22" s="194"/>
       <c r="K22" s="152"/>
       <c r="L22" s="152"/>
       <c r="M22" s="152"/>
@@ -3122,114 +3122,114 @@
     </row>
     <row r="23" spans="1:19" ht="30" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="181"/>
-      <c r="C23" s="181"/>
-      <c r="D23" s="181"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
-      <c r="G23" s="181"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="181"/>
+      <c r="B23" s="194"/>
+      <c r="C23" s="194"/>
+      <c r="D23" s="194"/>
+      <c r="E23" s="194"/>
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="194"/>
+      <c r="I23" s="194"/>
       <c r="J23" s="163"/>
       <c r="K23" s="151" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="164"/>
-      <c r="M23" s="183" t="s">
+      <c r="M23" s="196" t="s">
         <v>16</v>
       </c>
-      <c r="N23" s="183"/>
-      <c r="O23" s="183"/>
-      <c r="P23" s="173"/>
-      <c r="Q23" s="175" t="str">
+      <c r="N23" s="196"/>
+      <c r="O23" s="196"/>
+      <c r="P23" s="198"/>
+      <c r="Q23" s="200" t="str">
         <f>IF(COUNT(R8:R15)=8,MROUND(SUM(R8:R15)/SUM(Q8:Q15),0.5),"")</f>
         <v/>
       </c>
-      <c r="R23" s="176"/>
+      <c r="R23" s="201"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="181"/>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
+      <c r="B24" s="194"/>
+      <c r="C24" s="194"/>
+      <c r="D24" s="194"/>
+      <c r="E24" s="194"/>
+      <c r="F24" s="194"/>
+      <c r="G24" s="194"/>
+      <c r="H24" s="194"/>
+      <c r="I24" s="194"/>
       <c r="J24" s="165"/>
       <c r="K24" s="152"/>
       <c r="L24" s="151"/>
       <c r="M24" s="151"/>
       <c r="N24" s="151"/>
       <c r="O24" s="166"/>
-      <c r="P24" s="174"/>
-      <c r="Q24" s="177"/>
-      <c r="R24" s="178"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="202"/>
+      <c r="R24" s="203"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="181"/>
-      <c r="C25" s="181"/>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="181"/>
-      <c r="I25" s="181"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="194"/>
+      <c r="F25" s="194"/>
+      <c r="G25" s="194"/>
+      <c r="H25" s="194"/>
+      <c r="I25" s="194"/>
       <c r="J25" s="163"/>
       <c r="K25" s="152"/>
       <c r="L25" s="164"/>
       <c r="M25" s="152"/>
       <c r="N25" s="167"/>
       <c r="O25" s="166"/>
-      <c r="P25" s="174"/>
-      <c r="Q25" s="177"/>
-      <c r="R25" s="178"/>
+      <c r="P25" s="199"/>
+      <c r="Q25" s="202"/>
+      <c r="R25" s="203"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="181"/>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="181"/>
+      <c r="B26" s="194"/>
+      <c r="C26" s="194"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="194"/>
+      <c r="F26" s="194"/>
+      <c r="G26" s="194"/>
+      <c r="H26" s="194"/>
+      <c r="I26" s="194"/>
       <c r="J26" s="165"/>
       <c r="K26" s="168"/>
       <c r="L26" s="152"/>
       <c r="M26" s="152"/>
       <c r="N26" s="167"/>
       <c r="O26" s="166"/>
-      <c r="P26" s="174"/>
-      <c r="Q26" s="177"/>
-      <c r="R26" s="178"/>
+      <c r="P26" s="199"/>
+      <c r="Q26" s="202"/>
+      <c r="R26" s="203"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
+      <c r="B27" s="194"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="194"/>
+      <c r="F27" s="194"/>
+      <c r="G27" s="194"/>
+      <c r="H27" s="194"/>
+      <c r="I27" s="194"/>
       <c r="J27" s="165"/>
       <c r="K27" s="168"/>
       <c r="L27" s="152"/>
       <c r="M27" s="152"/>
       <c r="N27" s="167"/>
       <c r="O27" s="166"/>
-      <c r="P27" s="174"/>
-      <c r="Q27" s="179"/>
-      <c r="R27" s="180"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="204"/>
+      <c r="R27" s="205"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="9.75" hidden="1" customHeight="1" thickBot="1">
@@ -3289,14 +3289,14 @@
     <row r="42" spans="1:19" ht="12.75"/>
     <row r="43" spans="1:19" ht="12.75"/>
     <row r="44" spans="1:19" ht="12.75">
-      <c r="L44" s="172"/>
-      <c r="M44" s="172"/>
-      <c r="N44" s="172"/>
+      <c r="L44" s="197"/>
+      <c r="M44" s="197"/>
+      <c r="N44" s="197"/>
     </row>
     <row r="45" spans="1:19" ht="12.75">
-      <c r="L45" s="172"/>
-      <c r="M45" s="172"/>
-      <c r="N45" s="172"/>
+      <c r="L45" s="197"/>
+      <c r="M45" s="197"/>
+      <c r="N45" s="197"/>
     </row>
     <row r="46" spans="1:19" ht="12.75"/>
     <row r="47" spans="1:19" ht="12.75"/>
@@ -3339,24 +3339,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="27">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L44:N45"/>
     <mergeCell ref="P23:P27"/>
     <mergeCell ref="Q23:R27"/>
@@ -3366,6 +3348,24 @@
     <mergeCell ref="B27:I27"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="M23:O23"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="Q23:R27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3598,6 +3598,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="dfa80de1-e9bb-4cf2-893d-d06220b3971a" xsi:nil="true"/>
@@ -3606,15 +3615,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3637,6 +3637,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BF4B0E-51C7-4A9A-BA9D-2F7282E7E156}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22D60CBD-0DCA-4864-A27F-F5E8DAC174CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3645,12 +3653,4 @@
     <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BF4B0E-51C7-4A9A-BA9D-2F7282E7E156}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>